<commit_message>
Device export add imei, serial number
</commit_message>
<xml_diff>
--- a/templates/export/device.xlsx
+++ b/templates/export/device.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nspiraappcbd/Documents/GitHub/traccar/templates/export/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sainathavadhuta/Documents/code/traccar/templates/export/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4858E1C4-FE39-D143-B9C4-1692F79EE0BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42660B30-922C-9248-87CD-2E44EDE03FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>", lastCell="N2")</t>
+          <t>", lastCell="P2")</t>
         </r>
       </text>
     </comment>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Device Id</t>
   </si>
@@ -185,6 +185,18 @@
   </si>
   <si>
     <t>${device.longitude}</t>
+  </si>
+  <si>
+    <t>IMEI</t>
+  </si>
+  <si>
+    <t>Serial Number</t>
+  </si>
+  <si>
+    <t>${device.imei}</t>
+  </si>
+  <si>
+    <t>${device.serialNumber}</t>
   </si>
 </sst>
 </file>
@@ -1202,9 +1214,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N995"/>
+  <dimension ref="A1:P995"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="158" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1220,11 +1234,13 @@
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="55.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="30" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" customWidth="1"/>
+    <col min="15" max="15" width="17.83203125" customWidth="1"/>
+    <col min="16" max="16" width="55.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="32" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1265,10 +1281,16 @@
         <v>9</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -1309,10 +1331,16 @@
         <v>22</v>
       </c>
       <c r="N2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>